<commit_message>
updated GpBCS s.c. cpmc VMpBCS 4.1 - updated version for code developer
</commit_message>
<xml_diff>
--- a/Exact results/DMRG.xlsx
+++ b/Exact results/DMRG.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4A150290-B21C-4ADE-9643-58EF84FAD28D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164D6A54-551D-47C6-9832-558B23E5C0CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -409,17 +409,17 @@
     <col min="6" max="6" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -427,7 +427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -447,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>12</v>
       </c>
@@ -467,7 +467,7 @@
         <v>7.4425227799999993E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8</v>
       </c>
@@ -487,7 +487,7 @@
         <v>7.0220171599999999E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -507,12 +507,20 @@
         <v>5.22692246E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -522,8 +530,16 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -533,8 +549,16 @@
       <c r="C12" s="1">
         <v>7.6567281899999999E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -544,8 +568,16 @@
       <c r="C13" s="1">
         <v>7.1054278800000001E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -556,12 +588,30 @@
         <v>5.7242312000000003E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -571,8 +621,16 @@
       <c r="C17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8</v>
       </c>
@@ -580,6 +638,14 @@
         <v>-49.361280000000001</v>
       </c>
       <c r="C18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>